<commit_message>
Go impl: complete reconcile feature
</commit_message>
<xml_diff>
--- a/zip-pkg-in-go/testdata/excel/pkg-test.xlsx
+++ b/zip-pkg-in-go/testdata/excel/pkg-test.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="41">
   <si>
     <t xml:space="preserve">FileName</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t xml:space="preserve">ContactInfo.Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">David2-Passport.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">David2</t>
   </si>
 </sst>
 </file>
@@ -256,19 +262,19 @@
   </sheetPr>
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="289" zoomScaleNormal="289" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="289" zoomScaleNormal="289" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.05"/>
@@ -418,21 +424,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="289" zoomScaleNormal="289" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.05"/>
@@ -562,14 +568,54 @@
         <v>31</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>40544</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>44197</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M2" r:id="rId1" display="david.smith@gmail.com"/>
     <hyperlink ref="M3" r:id="rId2" display="Linda.Chau@yahoo.com"/>
+    <hyperlink ref="M4" r:id="rId3" display="david.smith@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>